<commit_message>
- TextBox가 OwnerObject의 Theater 기준으로 생성되도록 수정
</commit_message>
<xml_diff>
--- a/Workspace/DataTable/TheaterTable.xlsx
+++ b/Workspace/DataTable/TheaterTable.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ta\Unity Projects\StiffBug\Workspace\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDCDFC0-E9A3-4C57-A69D-81CC936BBEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF2BFA73-AE1F-48AD-B388-3C0C78C1D9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1500" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1932" yWindow="2904" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EditorMenuTable" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>KeyAlias</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,11 +59,45 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TheaterType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SizeS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OwnerObject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;base&gt;테스트으으&lt;/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;base&gt;테스트으으!2&lt;/&gt;</t>
+  </si>
+  <si>
+    <t>Test_Character_Face</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Character_Face</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TheaterType</t>
+    <t>TheaterTest3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;base&gt;테스트으으!3&lt;/&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -71,29 +105,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OwnerObject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;base&gt;테스트으으&lt;/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;base&gt;테스트으으!2&lt;/&gt;</t>
+    <t>PlayerCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,7 +130,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -139,10 +158,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -423,13 +442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="17.19921875" customWidth="1"/>
     <col min="2" max="2" width="25.09765625" customWidth="1"/>
@@ -440,7 +459,7 @@
     <col min="7" max="7" width="16.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,50 +473,79 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>